<commit_message>
added price as Number to seed-club
</commit_message>
<xml_diff>
--- a/backend/seedsDB/files/clubs.xlsx
+++ b/backend/seedsDB/files/clubs.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="159">
   <si>
     <t xml:space="preserve">Tаблица 1</t>
   </si>
@@ -142,6 +142,9 @@
   </si>
   <si>
     <t xml:space="preserve">ДЕТРОЙТ VR, WARFACE VR, SKYWALKER VR, МАФИЯ VR, ПОЛИГОН VR, КОД ДЕЛЬТА VR, ЛОВЦЫ ПРИВИДЕНИЙ VR, ФИКСИКИ VR, КОСМИЧЕСКАЯ ОБОРОНА VR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HTC Vive, Valve Index, Windows Mixed Reality</t>
   </si>
   <si>
     <t xml:space="preserve">Engage VR Мозайка</t>
@@ -522,7 +525,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <name val="Helvetica Neue"/>
@@ -563,11 +566,6 @@
       <name val="Helvetica Neue"/>
       <family val="0"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Helvetica Neue"/>
-      <family val="0"/>
     </font>
     <font>
       <sz val="11"/>
@@ -632,7 +630,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -669,14 +667,6 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
@@ -697,24 +687,25 @@
   <dimension ref="A1:K23"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B15" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A15" activeCellId="0" sqref="A15"/>
-      <selection pane="bottomRight" activeCell="D2" activeCellId="0" sqref="D2"/>
+      <selection pane="topRight" activeCell="F1" activeCellId="0" sqref="F1"/>
+      <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="K5" activeCellId="0" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="3" min="1" style="1" width="15.9464285714286"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="20.0803571428571"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="15.9464285714286"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="19.3705357142857"/>
-    <col collapsed="false" hidden="false" max="8" min="7" style="1" width="15.9464285714286"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="37.5625"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="48.0758928571429"/>
-    <col collapsed="false" hidden="false" max="256" min="11" style="1" width="15.9464285714286"/>
-    <col collapsed="false" hidden="false" max="1025" min="257" style="0" width="15.9464285714286"/>
+    <col collapsed="false" hidden="false" max="3" min="1" style="1" width="15.59375"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="19.6071428571429"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="15.59375"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="18.8973214285714"/>
+    <col collapsed="false" hidden="false" max="8" min="7" style="1" width="15.59375"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="36.8526785714286"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="47.0089285714286"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="37.3258928571429"/>
+    <col collapsed="false" hidden="false" max="256" min="12" style="1" width="15.59375"/>
+    <col collapsed="false" hidden="false" max="1025" min="257" style="0" width="15.59375"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="27.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -730,6 +721,7 @@
       <c r="H1" s="3"/>
       <c r="I1" s="3"/>
       <c r="J1" s="0"/>
+      <c r="K1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="4"/>
@@ -866,7 +858,7 @@
         <v>38</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>20</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="44.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -874,25 +866,25 @@
         <v>4</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="G6" s="6" t="s">
         <v>35</v>
       </c>
       <c r="H6" s="6" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="I6" s="7" t="s">
         <v>37</v>
@@ -909,25 +901,25 @@
         <v>5</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E7" s="6" t="s">
         <v>14</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="G7" s="6" t="s">
         <v>35</v>
       </c>
       <c r="H7" s="6" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="I7" s="7" t="s">
         <v>37</v>
@@ -944,31 +936,31 @@
         <v>7</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="G8" s="6" t="s">
         <v>35</v>
       </c>
       <c r="H8" s="6" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="I8" s="6" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="K8" s="1" t="s">
         <v>20</v>
@@ -979,29 +971,29 @@
         <v>8</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="E9" s="6"/>
       <c r="F9" s="7" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="G9" s="6" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="H9" s="6" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="I9" s="6" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="K9" s="1" t="s">
         <v>30</v>
@@ -1012,34 +1004,34 @@
         <v>9</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="C10" s="8" t="s">
         <v>65</v>
       </c>
+      <c r="C10" s="6" t="s">
+        <v>66</v>
+      </c>
       <c r="D10" s="6" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="G10" s="6" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="H10" s="6" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="I10" s="7" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>20</v>
+        <v>39</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="32.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1047,31 +1039,31 @@
         <v>10</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="G11" s="6" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="H11" s="6" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="I11" s="7" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="K11" s="1" t="s">
         <v>20</v>
@@ -1082,34 +1074,34 @@
         <v>11</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="F12" s="9" t="s">
         <v>84</v>
       </c>
+      <c r="F12" s="8" t="s">
+        <v>85</v>
+      </c>
       <c r="G12" s="6" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H12" s="6" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="I12" s="7" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="K12" s="10" t="s">
         <v>89</v>
+      </c>
+      <c r="K12" s="1" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="44.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1117,34 +1109,34 @@
         <v>12</v>
       </c>
       <c r="B13" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="F13" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="G13" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="H13" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="I13" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="K13" s="1" t="s">
         <v>90</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="D13" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="E13" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="F13" s="9" t="s">
-        <v>93</v>
-      </c>
-      <c r="G13" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="H13" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="I13" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="J13" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="K13" s="1" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="44.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1152,34 +1144,34 @@
         <v>13</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="F14" s="9" t="s">
-        <v>99</v>
+        <v>84</v>
+      </c>
+      <c r="F14" s="8" t="s">
+        <v>100</v>
       </c>
       <c r="G14" s="6" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="H14" s="6" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="I14" s="7" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="44.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1187,34 +1179,34 @@
         <v>14</v>
       </c>
       <c r="B15" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="F15" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="G15" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="H15" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="I15" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="K15" s="1" t="s">
         <v>90</v>
-      </c>
-      <c r="C15" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="D15" s="6" t="s">
-        <v>103</v>
-      </c>
-      <c r="E15" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="F15" s="9" t="s">
-        <v>93</v>
-      </c>
-      <c r="G15" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="H15" s="6" t="s">
-        <v>104</v>
-      </c>
-      <c r="I15" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="J15" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="K15" s="1" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="44.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1222,31 +1214,31 @@
         <v>15</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="E16" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="E16" s="6" t="s">
         <v>24</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="G16" s="6" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="H16" s="6" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="I16" s="7" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="K16" s="1" t="s">
         <v>20</v>
@@ -1257,31 +1249,31 @@
         <v>16</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="E17" s="6" t="s">
         <v>24</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="G17" s="6" t="s">
         <v>26</v>
       </c>
       <c r="H17" s="6" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="I17" s="7" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="J17" s="0" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="K17" s="1" t="s">
         <v>20</v>
@@ -1292,31 +1284,31 @@
         <v>17</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="E18" s="6" t="s">
         <v>24</v>
       </c>
       <c r="F18" s="7" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="G18" s="6" t="s">
         <v>35</v>
       </c>
       <c r="H18" s="6" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="I18" s="7" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="J18" s="0" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="K18" s="1" t="s">
         <v>20</v>
@@ -1327,34 +1319,34 @@
         <v>18</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="E19" s="6" t="s">
         <v>24</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="G19" s="6" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="H19" s="6" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="I19" s="7" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="J19" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="K19" s="1" t="s">
-        <v>20</v>
+        <v>39</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="44.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1362,31 +1354,31 @@
         <v>19</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="E20" s="6" t="s">
         <v>24</v>
       </c>
       <c r="F20" s="7" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="G20" s="6" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="H20" s="6" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="I20" s="7" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="K20" s="1" t="s">
         <v>20</v>
@@ -1397,31 +1389,31 @@
         <v>20</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="E21" s="6" t="s">
         <v>24</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="G21" s="6" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="H21" s="6" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="I21" s="7" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="K21" s="1" t="s">
         <v>20</v>
@@ -1432,31 +1424,31 @@
         <v>21</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="E22" s="6" t="s">
         <v>24</v>
       </c>
       <c r="F22" s="7" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="G22" s="6" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="H22" s="6" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="I22" s="7" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="K22" s="1" t="s">
         <v>20</v>
@@ -1467,31 +1459,31 @@
         <v>22</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="E23" s="6" t="s">
         <v>24</v>
       </c>
       <c r="F23" s="7" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="G23" s="6" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="H23" s="6" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="I23" s="7" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="J23" s="1" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="K23" s="1" t="s">
         <v>20</v>

</xml_diff>